<commit_message>
updated data for 8/22
</commit_message>
<xml_diff>
--- a/data/UniversityCovidData.xlsx
+++ b/data/UniversityCovidData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmg3\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neang/Documents/university-covid19-tracking/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10942A7-4A2C-4C3F-8084-141A98D7F884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF781B5-49BB-2D49-9E70-4EAB8E684B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{369D53F0-7860-4566-A341-53E379050634}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{369D53F0-7860-4566-A341-53E379050634}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,19 +477,19 @@
   <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -505,7 +505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -513,7 +513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -521,7 +521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -529,7 +529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -537,7 +537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -545,7 +545,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -562,7 +562,7 @@
         <v>44064</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -579,7 +579,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -596,7 +596,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
@@ -613,7 +613,7 @@
         <v>44059</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -630,7 +630,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -647,7 +647,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -668,7 +668,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -689,7 +689,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>2</v>
       </c>
@@ -760,7 +760,7 @@
         <v>44064</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
@@ -822,7 +822,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
@@ -884,7 +884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -966,7 +966,7 @@
       </c>
       <c r="U22" s="4"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="U23" s="4"/>
     </row>
-    <row r="25" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>20</v>
       </c>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>44062</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>11</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>44058</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>6370</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>20</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>6370</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>18</v>
       </c>
@@ -1581,8 +1581,11 @@
         <f t="shared" si="2"/>
         <v>44064</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q43" s="6">
+        <v>44065</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>10</v>
       </c>
@@ -1631,8 +1634,11 @@
       <c r="P44">
         <v>1016</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q44">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>11</v>
       </c>
@@ -1681,8 +1687,11 @@
       <c r="P45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>6</v>
       </c>
@@ -1746,8 +1755,12 @@
         <f>SUM($B$44:P44)</f>
         <v>4384</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q46">
+        <f>SUM($B$44:Q44)</f>
+        <v>5386</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -1809,6 +1822,10 @@
       </c>
       <c r="P47">
         <f>SUM($B$45:P45)</f>
+        <v>5</v>
+      </c>
+      <c r="Q47">
+        <f>SUM($B$45:Q45)</f>
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update testing numbers for 8/24
</commit_message>
<xml_diff>
--- a/data/UniversityCovidData.xlsx
+++ b/data/UniversityCovidData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmg3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38C1432-8269-4CBA-B4EC-C4E135D6FCAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FEE253-85D1-4FED-B420-AEFD38D838A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,45 +651,50 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>30101</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <f>3696+8287</f>
         <v>11983</v>
       </c>
-      <c r="F2">
-        <f>B2*D2+C2*E2</f>
+      <c r="F3">
+        <f>B3*D3+C3*E3</f>
         <v>42084</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2191,6 +2196,9 @@
       <c r="E54" s="3">
         <v>44064</v>
       </c>
+      <c r="F54" s="3">
+        <v>44067</v>
+      </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
@@ -2213,6 +2221,9 @@
       <c r="E56">
         <v>5</v>
       </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
@@ -2234,6 +2245,10 @@
         <f>SUM($B$55:E55)</f>
         <v>0</v>
       </c>
+      <c r="F57" s="5">
+        <f>SUM($B$55:F55)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
@@ -2255,6 +2270,10 @@
         <f>SUM($B$55:E56)</f>
         <v>10</v>
       </c>
+      <c r="F58" s="5">
+        <f>SUM($B$55:F56)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
@@ -2278,6 +2297,9 @@
       <c r="G60" s="3">
         <v>44066</v>
       </c>
+      <c r="H60" s="3">
+        <v>44067</v>
+      </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
@@ -2301,6 +2323,9 @@
       <c r="G61">
         <v>518</v>
       </c>
+      <c r="H61">
+        <v>6</v>
+      </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
@@ -2324,6 +2349,9 @@
       <c r="G62">
         <v>1</v>
       </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
@@ -2353,6 +2381,10 @@
         <f>SUM($B$61:G61)</f>
         <v>4683</v>
       </c>
+      <c r="H63" s="5">
+        <f>SUM($B$61:H61)</f>
+        <v>4689</v>
+      </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
@@ -2380,6 +2412,10 @@
       </c>
       <c r="G64" s="5">
         <f>SUM($B$62:G62)</f>
+        <v>7</v>
+      </c>
+      <c r="H64" s="5">
+        <f>SUM($B$62:H62)</f>
         <v>7</v>
       </c>
     </row>
@@ -3252,17 +3288,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{B9B804B5-EEBA-44B9-9BCD-FCE4B82EF109}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{70B9572E-6476-4A71-A002-798C5304CA81}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{00964D12-76B2-40D1-8EAA-437B78CA47E6}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{39AF576B-3B56-47BD-80CD-F90C4B49504E}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId7" xr:uid="{B9B804B5-EEBA-44B9-9BCD-FCE4B82EF109}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{70B9572E-6476-4A71-A002-798C5304CA81}"/>
+    <hyperlink ref="G11" r:id="rId9" xr:uid="{00964D12-76B2-40D1-8EAA-437B78CA47E6}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{39AF576B-3B56-47BD-80CD-F90C4B49504E}"/>
+    <hyperlink ref="G2" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>

</xml_diff>

<commit_message>
Update UNC Chapel Hill numbers
</commit_message>
<xml_diff>
--- a/data/UniversityCovidData.xlsx
+++ b/data/UniversityCovidData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmg3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8218F00C-B07D-44FB-9089-9FE84DE2CF60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019ECA13-A6C3-4A57-9008-2F4D7BF09F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110:V110"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,6 +937,9 @@
       <c r="E24" s="3">
         <v>44059</v>
       </c>
+      <c r="F24" s="3">
+        <v>44066</v>
+      </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -954,6 +957,9 @@
       <c r="E25">
         <v>954</v>
       </c>
+      <c r="F25">
+        <v>1568</v>
+      </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -971,6 +977,9 @@
       <c r="E26">
         <v>130</v>
       </c>
+      <c r="F26">
+        <v>505</v>
+      </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -992,6 +1001,10 @@
         <f>SUM(B25:E25)</f>
         <v>1583</v>
       </c>
+      <c r="F27" s="5">
+        <f>SUM(C25:F25)</f>
+        <v>3034</v>
+      </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -1012,6 +1025,10 @@
       <c r="E28">
         <f>SUM(B26:E26)</f>
         <v>166</v>
+      </c>
+      <c r="F28" s="5">
+        <f>SUM(C26:F26)</f>
+        <v>658</v>
       </c>
     </row>
     <row r="30" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add population sizes for each universities
</commit_message>
<xml_diff>
--- a/data/UniversityCovidData.xlsx
+++ b/data/UniversityCovidData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmg3\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neang/Documents/university-covid19-tracking/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE20D7D-95CF-444B-BD12-B78C02632E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B47E205-FACF-B14C-AD52-C86E9333039B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29200" windowHeight="19440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,33 +651,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="8" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="8" width="9.5" customWidth="1"/>
     <col min="9" max="16" width="9.6640625" customWidth="1"/>
-    <col min="17" max="20" width="9.5546875" customWidth="1"/>
-    <col min="21" max="21" width="10.109375" customWidth="1"/>
-    <col min="22" max="31" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="39" width="8.77734375" customWidth="1"/>
-    <col min="40" max="40" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="62" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="71" width="8.77734375" customWidth="1"/>
-    <col min="72" max="83" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="84" max="86" width="8.77734375" customWidth="1"/>
-    <col min="87" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="89" max="90" width="8.77734375" customWidth="1"/>
-    <col min="91" max="91" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="92" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="17" max="20" width="9.5" customWidth="1"/>
+    <col min="21" max="21" width="10.1640625" customWidth="1"/>
+    <col min="22" max="31" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="39" width="8.83203125" customWidth="1"/>
+    <col min="40" max="40" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="62" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="71" width="8.83203125" customWidth="1"/>
+    <col min="72" max="83" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="86" width="8.83203125" customWidth="1"/>
+    <col min="87" max="88" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="90" width="8.83203125" customWidth="1"/>
+    <col min="91" max="91" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="92" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
@@ -700,20 +700,32 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>36304</v>
+      </c>
+      <c r="E2" s="5">
+        <f>2336+6773</f>
+        <v>9109</v>
+      </c>
+      <c r="F2" s="5">
+        <f t="shared" ref="F2" si="0">B2*D2+C2*E2</f>
+        <v>45413</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -738,135 +750,398 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <f>8731+3950</f>
+        <v>12681</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1396</v>
+      </c>
+      <c r="F4" s="5">
+        <f>B4*D4+C4*E4</f>
+        <v>14077</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>96408</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8864</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" ref="F5:F19" si="1">B5*D5+C5*E5</f>
+        <v>105272</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>43411</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3055</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="1"/>
+        <v>46466</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>15634</v>
+      </c>
+      <c r="E7" s="5">
+        <v>41206</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="1"/>
+        <v>56840</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>30593</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1300</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="1"/>
+        <v>31893</v>
+      </c>
       <c r="G8" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>22850</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1563</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="1"/>
+        <v>24413</v>
+      </c>
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>41200</v>
+      </c>
+      <c r="E10" s="5">
+        <f>4610+5481</f>
+        <v>10091</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="1"/>
+        <v>51291</v>
+      </c>
       <c r="G10" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>46002</v>
+      </c>
+      <c r="E11" s="5">
+        <f>6771+18986</f>
+        <v>25757</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="1"/>
+        <v>71759</v>
+      </c>
       <c r="G11" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>51090</v>
+      </c>
+      <c r="E12" s="5">
+        <f>3722+11645</f>
+        <v>15367</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>66457</v>
+      </c>
       <c r="G12" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>36489</v>
+      </c>
+      <c r="E13" s="5">
+        <f>-1740+5923</f>
+        <v>4183</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>40672</v>
+      </c>
       <c r="G13" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
+        <v>11878</v>
+      </c>
+      <c r="E14" s="5">
+        <v>3498</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="1"/>
+        <v>15376</v>
+      </c>
       <c r="G14" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>39126</v>
+      </c>
+      <c r="E15" s="5">
+        <f>1063</f>
+        <v>1063</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="1"/>
+        <v>40189</v>
+      </c>
       <c r="G15" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5">
+        <v>37677</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2497</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="1"/>
+        <v>40174</v>
+      </c>
       <c r="G16" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>13609</v>
+      </c>
+      <c r="E17" s="5">
+        <v>4410</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="1"/>
+        <v>18019</v>
+      </c>
       <c r="G17" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
+        <v>7170</v>
+      </c>
+      <c r="E18" s="5">
+        <v>2832</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="1"/>
+        <v>10002</v>
+      </c>
       <c r="G18" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>41551</v>
+      </c>
+      <c r="E19" s="5">
+        <f>5966+8133</f>
+        <v>14099</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="1"/>
+        <v>55650</v>
+      </c>
       <c r="G19" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -889,7 +1164,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -912,7 +1187,7 @@
         <v>3031</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
@@ -935,7 +1210,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -955,7 +1230,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -975,7 +1250,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -995,7 +1270,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
@@ -1020,7 +1295,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -1045,7 +1320,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -1080,39 +1355,39 @@
         <v>44055</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" ref="L31:T31" si="0">K31+1</f>
+        <f t="shared" ref="L31:T31" si="2">K31+1</f>
         <v>44056</v>
       </c>
       <c r="M31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44057</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44058</v>
       </c>
       <c r="O31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44059</v>
       </c>
       <c r="P31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44060</v>
       </c>
       <c r="Q31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44061</v>
       </c>
       <c r="R31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44062</v>
       </c>
       <c r="S31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44063</v>
       </c>
       <c r="T31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44064</v>
       </c>
       <c r="U31" s="3">
@@ -1122,7 +1397,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -1190,7 +1465,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
@@ -1258,7 +1533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>14</v>
       </c>
@@ -1347,7 +1622,7 @@
         <v>2698</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>15</v>
       </c>
@@ -1436,7 +1711,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="37" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1447,7 +1722,7 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -1458,7 +1733,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>17</v>
       </c>
@@ -1469,7 +1744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>18</v>
       </c>
@@ -1483,7 +1758,7 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>19</v>
       </c>
@@ -1496,7 +1771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
@@ -1504,75 +1779,75 @@
         <v>44044</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" ref="C43:T43" si="1">B43+1</f>
+        <f t="shared" ref="C43:T43" si="3">B43+1</f>
         <v>44045</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44046</v>
       </c>
       <c r="E43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44047</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44048</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44049</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44050</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44051</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44052</v>
       </c>
       <c r="K43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44053</v>
       </c>
       <c r="L43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44054</v>
       </c>
       <c r="M43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44055</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44056</v>
       </c>
       <c r="O43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44057</v>
       </c>
       <c r="P43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44058</v>
       </c>
       <c r="Q43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44059</v>
       </c>
       <c r="R43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44060</v>
       </c>
       <c r="S43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44061</v>
       </c>
       <c r="T43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44062</v>
       </c>
       <c r="U43" s="3">
@@ -1585,7 +1860,7 @@
         <v>44065</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>20</v>
       </c>
@@ -1656,7 +1931,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>21</v>
       </c>
@@ -1727,7 +2002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>14</v>
       </c>
@@ -1820,7 +2095,7 @@
         <v>2947</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>15</v>
       </c>
@@ -1913,7 +2188,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -1924,7 +2199,7 @@
         <v>44064</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>16</v>
       </c>
@@ -1936,7 +2211,7 @@
         <v>5028</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>17</v>
       </c>
@@ -1948,7 +2223,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>18</v>
       </c>
@@ -1961,7 +2236,7 @@
         <v>11398</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>19</v>
       </c>
@@ -1974,7 +2249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>12</v>
       </c>
@@ -1982,59 +2257,59 @@
         <v>44050</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" ref="C55:P55" si="2">B55+1</f>
+        <f t="shared" ref="C55:P55" si="4">B55+1</f>
         <v>44051</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44052</v>
       </c>
       <c r="E55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44053</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44054</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44055</v>
       </c>
       <c r="H55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44056</v>
       </c>
       <c r="I55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44057</v>
       </c>
       <c r="J55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44058</v>
       </c>
       <c r="K55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44059</v>
       </c>
       <c r="L55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44060</v>
       </c>
       <c r="M55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44061</v>
       </c>
       <c r="N55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44062</v>
       </c>
       <c r="O55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44063</v>
       </c>
       <c r="P55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44064</v>
       </c>
       <c r="Q55" s="3">
@@ -2044,7 +2319,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>20</v>
       </c>
@@ -2100,7 +2375,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>21</v>
       </c>
@@ -2156,7 +2431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>14</v>
       </c>
@@ -2229,7 +2504,7 @@
         <v>6053</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>15</v>
       </c>
@@ -2302,7 +2577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>22</v>
       </c>
@@ -2322,12 +2597,12 @@
         <v>44067</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>17</v>
       </c>
@@ -2347,7 +2622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>18</v>
       </c>
@@ -2372,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>19</v>
       </c>
@@ -2397,7 +2672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>24</v>
       </c>
@@ -2423,7 +2698,7 @@
         <v>44067</v>
       </c>
     </row>
-    <row r="68" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>20</v>
       </c>
@@ -2449,7 +2724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>21</v>
       </c>
@@ -2475,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>14</v>
       </c>
@@ -2508,7 +2783,7 @@
         <v>4689</v>
       </c>
     </row>
-    <row r="71" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>15</v>
       </c>
@@ -2541,7 +2816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>26</v>
       </c>
@@ -2549,105 +2824,105 @@
         <v>43898</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" ref="C73:Z73" si="3">B73+7</f>
+        <f t="shared" ref="C73:Z73" si="5">B73+7</f>
         <v>43905</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43912</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43919</v>
       </c>
       <c r="F73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43926</v>
       </c>
       <c r="G73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43933</v>
       </c>
       <c r="H73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43940</v>
       </c>
       <c r="I73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43947</v>
       </c>
       <c r="J73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43954</v>
       </c>
       <c r="K73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43961</v>
       </c>
       <c r="L73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43968</v>
       </c>
       <c r="M73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43975</v>
       </c>
       <c r="N73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43982</v>
       </c>
       <c r="O73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43989</v>
       </c>
       <c r="P73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>43996</v>
       </c>
       <c r="Q73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44003</v>
       </c>
       <c r="R73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44010</v>
       </c>
       <c r="S73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44017</v>
       </c>
       <c r="T73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44024</v>
       </c>
       <c r="U73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44031</v>
       </c>
       <c r="V73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44038</v>
       </c>
       <c r="W73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44045</v>
       </c>
       <c r="X73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44052</v>
       </c>
       <c r="Y73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44059</v>
       </c>
       <c r="Z73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44066</v>
       </c>
       <c r="AA73" s="3"/>
       <c r="AB73" s="3"/>
     </row>
-    <row r="74" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>16</v>
       </c>
@@ -2727,7 +3002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>28</v>
       </c>
@@ -2807,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>17</v>
       </c>
@@ -2816,103 +3091,103 @@
         <v>7</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" ref="C76:Z76" si="4">ROUND(C75*C74,0)</f>
+        <f t="shared" ref="C76:Z76" si="6">ROUND(C75*C74,0)</f>
         <v>34</v>
       </c>
       <c r="D76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="E76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="F76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="G76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="M76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="N76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="P76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="Q76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="R76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="S76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="T76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="U76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="V76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="W76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="X76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="Y76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="Z76" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:95" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>18</v>
       </c>
@@ -3017,7 +3292,7 @@
         <v>8252</v>
       </c>
     </row>
-    <row r="78" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>19</v>
       </c>
@@ -3122,7 +3397,7 @@
         <v>1.2409999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:95" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>29</v>
       </c>
@@ -3149,19 +3424,19 @@
         <v>44031</v>
       </c>
       <c r="H80" s="3">
-        <f t="shared" ref="H80:K80" si="5">G80+7</f>
+        <f t="shared" ref="H80:K80" si="7">G80+7</f>
         <v>44038</v>
       </c>
       <c r="I80" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44045</v>
       </c>
       <c r="J80" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44052</v>
       </c>
       <c r="K80" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44059</v>
       </c>
       <c r="M80" s="3"/>
@@ -3248,7 +3523,7 @@
       <c r="CP80" s="3"/>
       <c r="CQ80" s="3"/>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
@@ -3283,7 +3558,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>17</v>
       </c>
@@ -3318,7 +3593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>18</v>
       </c>
@@ -3363,7 +3638,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>19</v>
       </c>
@@ -3408,7 +3683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>38</v>
       </c>
@@ -3420,59 +3695,59 @@
         <v>44053</v>
       </c>
       <c r="D86" s="3">
-        <f t="shared" ref="D86:P86" si="6">C86+1</f>
+        <f t="shared" ref="D86:P86" si="8">C86+1</f>
         <v>44054</v>
       </c>
       <c r="E86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44055</v>
       </c>
       <c r="F86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44056</v>
       </c>
       <c r="G86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44057</v>
       </c>
       <c r="H86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44058</v>
       </c>
       <c r="I86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44059</v>
       </c>
       <c r="J86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44060</v>
       </c>
       <c r="K86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44061</v>
       </c>
       <c r="L86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44062</v>
       </c>
       <c r="M86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44063</v>
       </c>
       <c r="N86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44064</v>
       </c>
       <c r="O86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44065</v>
       </c>
       <c r="P86" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44066</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>20</v>
       </c>
@@ -3522,32 +3797,32 @@
         <v>225</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B88">
-        <f t="shared" ref="B88:G88" si="7">16/6</f>
+        <f t="shared" ref="B88:G88" si="9">16/6</f>
         <v>2.6666666666666665</v>
       </c>
       <c r="C88" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="D88" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="E88" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="F88" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="G88" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="H88">
@@ -3578,7 +3853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>14</v>
       </c>
@@ -3643,7 +3918,7 @@
         <v>11025</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>15</v>
       </c>
@@ -3708,7 +3983,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>40</v>
       </c>
@@ -3716,7 +3991,7 @@
         <v>44067</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>14</v>
       </c>
@@ -3724,7 +3999,7 @@
         <v>5333</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>15</v>
       </c>
@@ -3732,7 +4007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>44</v>
       </c>
@@ -3740,89 +4015,89 @@
         <v>44045</v>
       </c>
       <c r="C96" s="3">
-        <f t="shared" ref="C96:V96" si="8">B96+1</f>
+        <f t="shared" ref="C96:V96" si="10">B96+1</f>
         <v>44046</v>
       </c>
       <c r="D96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44047</v>
       </c>
       <c r="E96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44048</v>
       </c>
       <c r="F96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44049</v>
       </c>
       <c r="G96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44050</v>
       </c>
       <c r="H96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44051</v>
       </c>
       <c r="I96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44052</v>
       </c>
       <c r="J96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44053</v>
       </c>
       <c r="K96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44054</v>
       </c>
       <c r="L96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44055</v>
       </c>
       <c r="M96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44056</v>
       </c>
       <c r="N96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44057</v>
       </c>
       <c r="O96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44058</v>
       </c>
       <c r="P96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44059</v>
       </c>
       <c r="Q96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44060</v>
       </c>
       <c r="R96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44061</v>
       </c>
       <c r="S96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44062</v>
       </c>
       <c r="T96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44063</v>
       </c>
       <c r="U96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44064</v>
       </c>
       <c r="V96" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>44065</v>
       </c>
       <c r="W96" s="3"/>
       <c r="X96" s="3"/>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>16</v>
       </c>
@@ -3839,96 +4114,96 @@
         <v>127</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B98">
-        <f t="shared" ref="B98:H98" si="9">$H$97/7</f>
+        <f t="shared" ref="B98:H98" si="11">$H$97/7</f>
         <v>63.142857142857146</v>
       </c>
       <c r="C98" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>63.142857142857146</v>
       </c>
       <c r="D98" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>63.142857142857146</v>
       </c>
       <c r="E98" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>63.142857142857146</v>
       </c>
       <c r="F98" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>63.142857142857146</v>
       </c>
       <c r="G98" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>63.142857142857146</v>
       </c>
       <c r="H98" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>63.142857142857146</v>
       </c>
       <c r="I98">
-        <f t="shared" ref="I98:O98" si="10">$O$97/7</f>
+        <f t="shared" ref="I98:O98" si="12">$O$97/7</f>
         <v>32.714285714285715</v>
       </c>
       <c r="J98" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32.714285714285715</v>
       </c>
       <c r="K98" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32.714285714285715</v>
       </c>
       <c r="L98" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32.714285714285715</v>
       </c>
       <c r="M98" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32.714285714285715</v>
       </c>
       <c r="N98" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32.714285714285715</v>
       </c>
       <c r="O98" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32.714285714285715</v>
       </c>
       <c r="P98">
-        <f t="shared" ref="P98:V98" si="11">$V$97/7</f>
+        <f t="shared" ref="P98:V98" si="13">$V$97/7</f>
         <v>18.142857142857142</v>
       </c>
       <c r="Q98" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.142857142857142</v>
       </c>
       <c r="R98" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.142857142857142</v>
       </c>
       <c r="S98" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.142857142857142</v>
       </c>
       <c r="T98" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.142857142857142</v>
       </c>
       <c r="U98" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.142857142857142</v>
       </c>
       <c r="V98" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.142857142857142</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>21</v>
       </c>
@@ -3996,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>14</v>
       </c>
@@ -4085,7 +4360,7 @@
         <v>797.99999999999966</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>15</v>
       </c>
@@ -4174,7 +4449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>46</v>
       </c>
@@ -4185,7 +4460,7 @@
         <v>44068</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>14</v>
       </c>
@@ -4196,7 +4471,7 @@
         <v>13623</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>15</v>
       </c>
@@ -4207,7 +4482,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>48</v>
       </c>
@@ -4227,75 +4502,75 @@
         <v>44049</v>
       </c>
       <c r="F107" s="3">
-        <f t="shared" ref="F107:V107" si="12">E107+1</f>
+        <f t="shared" ref="F107:V107" si="14">E107+1</f>
         <v>44050</v>
       </c>
       <c r="G107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44051</v>
       </c>
       <c r="H107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44052</v>
       </c>
       <c r="I107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44053</v>
       </c>
       <c r="J107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44054</v>
       </c>
       <c r="K107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44055</v>
       </c>
       <c r="L107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44056</v>
       </c>
       <c r="M107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44057</v>
       </c>
       <c r="N107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44058</v>
       </c>
       <c r="O107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44059</v>
       </c>
       <c r="P107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44060</v>
       </c>
       <c r="Q107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44061</v>
       </c>
       <c r="R107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44062</v>
       </c>
       <c r="S107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44063</v>
       </c>
       <c r="T107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44064</v>
       </c>
       <c r="U107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44065</v>
       </c>
       <c r="V107" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44066</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>20</v>
       </c>
@@ -4363,7 +4638,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>21</v>
       </c>
@@ -4431,7 +4706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>14</v>
       </c>
@@ -4520,7 +4795,7 @@
         <v>7230</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>15</v>
       </c>
@@ -4609,7 +4884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>50</v>
       </c>
@@ -4617,7 +4892,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>14</v>
       </c>
@@ -4625,7 +4900,7 @@
         <v>6630</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
update data files on 8/25
</commit_message>
<xml_diff>
--- a/data/UniversityCovidData.xlsx
+++ b/data/UniversityCovidData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neang/Documents/university-covid19-tracking/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B47E205-FACF-B14C-AD52-C86E9333039B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61329A41-5F15-564E-9DC6-20C102A8A7EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29200" windowHeight="19440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16060" windowHeight="19440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1068,7 +1068,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>48</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>50</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1163,8 +1163,11 @@
       <c r="G21" s="3">
         <v>44066</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="H21" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -1186,8 +1189,11 @@
       <c r="G22">
         <v>3031</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
@@ -1209,8 +1215,11 @@
       <c r="G23">
         <v>240</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1239,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +1279,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
@@ -1295,7 +1304,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -1320,7 +1329,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -1396,8 +1405,11 @@
       <c r="V31" s="3">
         <v>44066</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W31" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -1464,8 +1476,11 @@
       <c r="V32">
         <v>359</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W32">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
@@ -1532,8 +1547,11 @@
       <c r="V33">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>14</v>
       </c>
@@ -1621,8 +1639,12 @@
         <f>SUM($B$32:V32)</f>
         <v>2698</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W34" s="5">
+        <f>SUM($B$32:W32)</f>
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>15</v>
       </c>
@@ -1710,8 +1732,12 @@
         <f>SUM($B$33:V33)</f>
         <v>421</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W35" s="5">
+        <f>SUM($B$33:W33)</f>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1722,7 +1748,7 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -1733,7 +1759,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>17</v>
       </c>
@@ -1744,7 +1770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>18</v>
       </c>
@@ -1758,7 +1784,7 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>19</v>
       </c>
@@ -1771,7 +1797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
@@ -1859,8 +1885,11 @@
       <c r="W43" s="3">
         <v>44065</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X43" s="3">
+        <v>44066</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>20</v>
       </c>
@@ -1930,8 +1959,11 @@
       <c r="W44">
         <v>168</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X44">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>21</v>
       </c>
@@ -2001,8 +2033,11 @@
       <c r="W45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>14</v>
       </c>
@@ -2094,8 +2129,12 @@
         <f>SUM($B$44:W44)</f>
         <v>2947</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X46" s="5">
+        <f>SUM($B$44:X44)</f>
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>15</v>
       </c>
@@ -2187,8 +2226,12 @@
         <f>SUM($B$45:W45)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X47" s="5">
+        <f>SUM($B$45:X45)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -2199,7 +2242,7 @@
         <v>44064</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>16</v>
       </c>
@@ -2211,7 +2254,7 @@
         <v>5028</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>17</v>
       </c>
@@ -2223,7 +2266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>18</v>
       </c>
@@ -2236,7 +2279,7 @@
         <v>11398</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>19</v>
       </c>
@@ -2249,7 +2292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>12</v>
       </c>
@@ -2318,8 +2361,11 @@
       <c r="R55" s="3">
         <v>44066</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S55" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>20</v>
       </c>
@@ -2374,8 +2420,11 @@
       <c r="R56">
         <v>667</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S56">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>21</v>
       </c>
@@ -2430,8 +2479,11 @@
       <c r="R57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>14</v>
       </c>
@@ -2503,8 +2555,12 @@
         <f>SUM($B$56:R56)</f>
         <v>6053</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S58" s="5">
+        <f>SUM($B$56:S56)</f>
+        <v>6934</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>15</v>
       </c>
@@ -2576,8 +2632,12 @@
         <f>SUM($B$57:R57)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S59" s="5">
+        <f>SUM($B$57:S57)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>22</v>
       </c>
@@ -2597,12 +2657,12 @@
         <v>44067</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>17</v>
       </c>
@@ -2622,7 +2682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>18</v>
       </c>

</xml_diff>